<commit_message>
Udate material for qc
</commit_message>
<xml_diff>
--- a/IT002-OOP/Điểm thực hành/it002n21cttn/IT002.N21.CTTN.1.xlsx
+++ b/IT002-OOP/Điểm thực hành/it002n21cttn/IT002.N21.CTTN.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vutuanhai/Desktop/Quan trọng/CourseMaterials/IT002-OOP/Điểm thực hành/it002n21cttn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02B5E05-CCDD-374D-827A-A048EDEE5487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8C1C57-0378-704F-893C-2BD9768F65F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT002.N21.CTTN.1" sheetId="1" r:id="rId1"/>
@@ -601,22 +601,13 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -635,8 +626,17 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -962,11 +962,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="9"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -976,11 +976,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="1"/>
@@ -998,22 +998,22 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="35"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="14">
         <v>2</v>
       </c>
@@ -1032,10 +1032,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="34"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1052,10 +1052,10 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1072,10 +1072,10 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="34"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="4">
         <v>80503</v>
       </c>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="43">
+      <c r="F13" s="31">
         <v>7.125</v>
       </c>
       <c r="G13" s="22"/>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="43">
+      <c r="F14" s="31">
         <v>6.21875</v>
       </c>
       <c r="G14" s="22"/>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="23"/>
-      <c r="F15" s="43">
+      <c r="F15" s="31">
         <v>7.0250000000000004</v>
       </c>
       <c r="G15" s="22"/>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23"/>
-      <c r="F16" s="43">
+      <c r="F16" s="31">
         <v>5.65625</v>
       </c>
       <c r="G16" s="22"/>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="23"/>
-      <c r="F17" s="43">
+      <c r="F17" s="31">
         <v>6.3687500000000004</v>
       </c>
       <c r="G17" s="22"/>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="23"/>
-      <c r="F18" s="43">
+      <c r="F18" s="31">
         <v>6.9</v>
       </c>
       <c r="G18" s="22"/>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23"/>
-      <c r="F19" s="43">
+      <c r="F19" s="31">
         <v>6.1083375000000002</v>
       </c>
       <c r="G19" s="22"/>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="43">
+      <c r="F20" s="31">
         <v>4.25</v>
       </c>
       <c r="G20" s="22"/>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="23"/>
-      <c r="F21" s="43">
+      <c r="F21" s="31">
         <v>7.84375</v>
       </c>
       <c r="G21" s="22"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23"/>
-      <c r="F22" s="43">
+      <c r="F22" s="31">
         <v>6.6875</v>
       </c>
       <c r="G22" s="22"/>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="23"/>
-      <c r="F23" s="43">
+      <c r="F23" s="31">
         <v>5.4937500000000004</v>
       </c>
       <c r="G23" s="22"/>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="23"/>
-      <c r="F24" s="43">
+      <c r="F24" s="31">
         <v>6.25</v>
       </c>
       <c r="G24" s="22"/>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="23"/>
-      <c r="F25" s="43">
+      <c r="F25" s="31">
         <v>5.75</v>
       </c>
       <c r="G25" s="22"/>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="23"/>
-      <c r="F26" s="43">
+      <c r="F26" s="31">
         <v>5.8406250000000002</v>
       </c>
       <c r="G26" s="22"/>
@@ -1472,7 +1472,7 @@
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="23"/>
-      <c r="F27" s="43">
+      <c r="F27" s="31">
         <v>6.53125</v>
       </c>
       <c r="G27" s="22"/>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="23"/>
-      <c r="F28" s="43">
+      <c r="F28" s="31">
         <v>6.6666624999999993</v>
       </c>
       <c r="G28" s="22"/>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="23"/>
-      <c r="F29" s="43">
+      <c r="F29" s="31">
         <v>4.95</v>
       </c>
       <c r="G29" s="22"/>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="43">
+      <c r="F30" s="31">
         <v>6.3687500000000004</v>
       </c>
       <c r="G30" s="22"/>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="43">
+      <c r="F31" s="31">
         <v>4.5</v>
       </c>
       <c r="G31" s="22"/>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="43">
+      <c r="F32" s="31">
         <v>5.8250000000000002</v>
       </c>
       <c r="G32" s="22"/>
@@ -1598,7 +1598,7 @@
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="23"/>
-      <c r="F33" s="43">
+      <c r="F33" s="31">
         <v>6.25</v>
       </c>
       <c r="G33" s="22"/>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="D34" s="22"/>
       <c r="E34" s="23"/>
-      <c r="F34" s="43">
+      <c r="F34" s="31">
         <v>6.3250000000000002</v>
       </c>
       <c r="G34" s="22"/>
@@ -1640,7 +1640,7 @@
       </c>
       <c r="D35" s="22"/>
       <c r="E35" s="23"/>
-      <c r="F35" s="43">
+      <c r="F35" s="31">
         <v>6.0750000000000002</v>
       </c>
       <c r="G35" s="22"/>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="43">
+      <c r="F36" s="31">
         <v>5.9187500000000002</v>
       </c>
       <c r="G36" s="22"/>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="D37" s="22"/>
       <c r="E37" s="23"/>
-      <c r="F37" s="43">
+      <c r="F37" s="31">
         <v>3.265625</v>
       </c>
       <c r="G37" s="22"/>
@@ -1703,8 +1703,8 @@
       </c>
       <c r="D38" s="22"/>
       <c r="E38" s="23"/>
-      <c r="F38" s="43">
-        <v>1.28125</v>
+      <c r="F38" s="31">
+        <v>5.5</v>
       </c>
       <c r="G38" s="22"/>
       <c r="H38" s="24"/>
@@ -1724,7 +1724,7 @@
       </c>
       <c r="D39" s="22"/>
       <c r="E39" s="23"/>
-      <c r="F39" s="43">
+      <c r="F39" s="31">
         <v>3.2083375000000003</v>
       </c>
       <c r="G39" s="22"/>
@@ -1745,7 +1745,7 @@
       </c>
       <c r="D40" s="22"/>
       <c r="E40" s="23"/>
-      <c r="F40" s="43">
+      <c r="F40" s="31">
         <v>9</v>
       </c>
       <c r="G40" s="22"/>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="D41" s="22"/>
       <c r="E41" s="23"/>
-      <c r="F41" s="43">
+      <c r="F41" s="31">
         <v>4.375</v>
       </c>
       <c r="G41" s="22"/>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D42" s="22"/>
       <c r="E42" s="23"/>
-      <c r="F42" s="43">
+      <c r="F42" s="31">
         <v>6.8125</v>
       </c>
       <c r="G42" s="22"/>
@@ -1811,49 +1811,49 @@
       <c r="A44" s="12"/>
       <c r="B44" s="25"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="38"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="D45" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="40"/>
-      <c r="F45" s="41" t="s">
+      <c r="E45" s="37"/>
+      <c r="F45" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A46" s="42" t="s">
+      <c r="A46" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="42"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="D46" s="42" t="s">
+      <c r="D46" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42" t="s">
+      <c r="E46" s="39"/>
+      <c r="F46" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
     </row>
     <row r="47" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
@@ -1881,47 +1881,52 @@
       <c r="A50" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="17">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="B50:H50"/>
     <mergeCell ref="B51:H51"/>
     <mergeCell ref="A7:B7"/>
@@ -1934,11 +1939,6 @@
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="F46:H46"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.26" right="0.17" top="0.32" bottom="0.28999999999999998" header="0.25" footer="0.19"/>
   <pageSetup orientation="portrait"/>

</xml_diff>